<commit_message>
updates to code with movie trends
</commit_message>
<xml_diff>
--- a/code/Data/tagged/data_mining_viable_data.xlsx
+++ b/code/Data/tagged/data_mining_viable_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionmail-my.sharepoint.com/personal/nirgutman212_campus_technion_ac_il/Documents/Courses/Semester 12/Advanced Signal Processing/Project/myCode/Data/tagged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{DC94D106-9EBE-4E12-8F2B-614586DF3C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C979F0F4-A4A9-4F28-B871-77644BDE17E5}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{DC94D106-9EBE-4E12-8F2B-614586DF3C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0104104-F658-4268-9DAF-51810F5E5D62}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-6495" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="29">
   <si>
     <t>label1</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>00007004_s006_t000</t>
+  </si>
+  <si>
+    <t>RightStroke</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,6 +938,146 @@
         <v>23</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="5">
+        <v>350000</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1700000</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -939,15 +1085,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042CD88665544244CB8A518F334EBA660" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2729e9abe74eb742b3c2b201d27423a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc679c0a-10ca-4006-b255-fa7e7faef444" xmlns:ns4="7f9ce069-e6c0-4690-98c3-882f05602da4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="794014e83e689c0f9656436de291e921" ns3:_="" ns4:_="">
     <xsd:import namespace="fc679c0a-10ca-4006-b255-fa7e7faef444"/>
@@ -1176,6 +1313,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1183,14 +1329,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02DB0CF1-9C6D-4198-959C-B97FEB52FD5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3355FE57-C66A-4BF0-89B5-E1CC4B6D32AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1205,6 +1343,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02DB0CF1-9C6D-4198-959C-B97FEB52FD5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
The version that was used for presentation
</commit_message>
<xml_diff>
--- a/code/Data/tagged/data_mining_viable_data.xlsx
+++ b/code/Data/tagged/data_mining_viable_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionmail-my.sharepoint.com/personal/nirgutman212_campus_technion_ac_il/Documents/Courses/Semester 12/Advanced Signal Processing/Project/myCode/Data/tagged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{DC94D106-9EBE-4E12-8F2B-614586DF3C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0104104-F658-4268-9DAF-51810F5E5D62}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{DC94D106-9EBE-4E12-8F2B-614586DF3C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA89C6A7-B7B3-4623-A847-15DC29D4DD7B}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-6495" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="37">
   <si>
     <t>label1</t>
   </si>
@@ -112,6 +112,30 @@
   </si>
   <si>
     <t>RightStroke</t>
+  </si>
+  <si>
+    <t>00015021_s001_t000</t>
+  </si>
+  <si>
+    <t>Nan</t>
+  </si>
+  <si>
+    <t>00013634_s002_t000</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>00013547_s001_t001</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -150,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -158,11 +182,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -181,6 +214,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +846,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C17" s="4">
         <v>25000</v>
@@ -823,7 +866,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4">
         <v>25000</v>
@@ -843,7 +886,7 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4">
         <v>25000</v>
@@ -863,7 +906,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4">
         <v>25000</v>
@@ -883,7 +926,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4">
         <v>25000</v>
@@ -903,7 +946,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4">
         <v>25000</v>
@@ -923,7 +966,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4">
         <v>25000</v>
@@ -1076,6 +1119,446 @@
       </c>
       <c r="F30" s="5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5">
+        <v>55000</v>
+      </c>
+      <c r="D31" s="5">
+        <v>310000</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="5">
+        <v>55000</v>
+      </c>
+      <c r="D32" s="5">
+        <v>310000</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5">
+        <v>55000</v>
+      </c>
+      <c r="D33" s="5">
+        <v>310000</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D34" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D35" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D36" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D37" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D38" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D39" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D40" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D41" s="4">
+        <v>300000</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="10">
+        <v>100000</v>
+      </c>
+      <c r="D42" s="10">
+        <v>300000</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D43" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D44" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D45" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D46" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D47" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D48" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D49" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D50" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D51" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="8">
+        <v>35000</v>
+      </c>
+      <c r="D52" s="8">
+        <v>305000</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1085,6 +1568,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042CD88665544244CB8A518F334EBA660" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2729e9abe74eb742b3c2b201d27423a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc679c0a-10ca-4006-b255-fa7e7faef444" xmlns:ns4="7f9ce069-e6c0-4690-98c3-882f05602da4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="794014e83e689c0f9656436de291e921" ns3:_="" ns4:_="">
     <xsd:import namespace="fc679c0a-10ca-4006-b255-fa7e7faef444"/>
@@ -1313,22 +1811,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6587A6-5430-4586-8324-0BDADFF8102B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7f9ce069-e6c0-4690-98c3-882f05602da4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc679c0a-10ca-4006-b255-fa7e7faef444"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02DB0CF1-9C6D-4198-959C-B97FEB52FD5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3355FE57-C66A-4BF0-89B5-E1CC4B6D32AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1345,29 +1853,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02DB0CF1-9C6D-4198-959C-B97FEB52FD5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6587A6-5430-4586-8324-0BDADFF8102B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7f9ce069-e6c0-4690-98c3-882f05602da4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fc679c0a-10ca-4006-b255-fa7e7faef444"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>